<commit_message>
adding pulse ox profile
</commit_message>
<xml_diff>
--- a/source/source_spreadsheets/uscdi_table.xlsx
+++ b/source/source_spreadsheets/uscdi_table.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core-R4/source/source_spreadsheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ERICS-AIR-2\ehaas\Documents\FHIR\Argo-R4\source\source_spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F2EC43E5-C7B2-5F44-A6BB-DB94DBF4F2AC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7706B949-5C70-4216-A639-85AB19E4D562}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{AF8CF676-F508-9E49-96CF-11F4326F15E6}"/>
+    <workbookView xWindow="375" yWindow="465" windowWidth="28035" windowHeight="17040" xr2:uid="{AF8CF676-F508-9E49-96CF-11F4326F15E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029" refMode="R1C1"/>
+  <calcPr calcId="191029" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -403,9 +402,6 @@
     <t>[Blood pressure systolic and diastolic] (From FHIR Core Profiles for Observation)</t>
   </si>
   <si>
-    <t>[Oxygen saturation] (From FHIR Core Profiles for Observation)</t>
-  </si>
-  <si>
     <t>[Head circumference] (From FHIR Core Profiles for Observation)</t>
   </si>
   <si>
@@ -413,6 +409,9 @@
   </si>
   <si>
     <t>DocumentReference</t>
+  </si>
+  <si>
+    <t>[US Core Pulse Oximetry Profile]</t>
   </si>
 </sst>
 </file>
@@ -797,17 +796,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01009508-76D3-D741-AF15-9B97E20050F9}">
   <dimension ref="A1:C59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C58" sqref="A1:C58"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="54.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="60.1640625" customWidth="1"/>
+    <col min="1" max="1" width="54.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="60.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" s="1" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -818,7 +817,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -829,7 +828,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -840,45 +839,45 @@
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C5" t="s">
         <v>125</v>
       </c>
-      <c r="C5" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>124</v>
+      </c>
+      <c r="C6" t="s">
         <v>125</v>
       </c>
-      <c r="C6" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>124</v>
+      </c>
+      <c r="C7" t="s">
         <v>125</v>
       </c>
-      <c r="C7" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -889,7 +888,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -900,7 +899,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -911,7 +910,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -922,7 +921,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -933,34 +932,34 @@
         <v>119</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
       <c r="B13" t="s">
+        <v>124</v>
+      </c>
+      <c r="C13" t="s">
         <v>125</v>
       </c>
-      <c r="C13" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>4</v>
       </c>
       <c r="B14" t="s">
+        <v>124</v>
+      </c>
+      <c r="C14" t="s">
         <v>125</v>
       </c>
-      <c r="C14" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -971,7 +970,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -982,7 +981,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -993,12 +992,12 @@
         <v>98</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -1006,7 +1005,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -1017,12 +1016,12 @@
         <v>92</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -1033,7 +1032,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -1044,14 +1043,14 @@
         <v>89</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>105</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>23</v>
       </c>
@@ -1062,7 +1061,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>24</v>
       </c>
@@ -1073,7 +1072,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>25</v>
       </c>
@@ -1084,7 +1083,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>26</v>
       </c>
@@ -1095,7 +1094,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>27</v>
       </c>
@@ -1106,7 +1105,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>28</v>
       </c>
@@ -1117,7 +1116,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>29</v>
       </c>
@@ -1128,7 +1127,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>30</v>
       </c>
@@ -1139,7 +1138,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>31</v>
       </c>
@@ -1150,7 +1149,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>32</v>
       </c>
@@ -1161,7 +1160,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>33</v>
       </c>
@@ -1172,7 +1171,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>34</v>
       </c>
@@ -1183,7 +1182,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>35</v>
       </c>
@@ -1194,7 +1193,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>36</v>
       </c>
@@ -1205,7 +1204,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>37</v>
       </c>
@@ -1216,7 +1215,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>38</v>
       </c>
@@ -1227,7 +1226,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>39</v>
       </c>
@@ -1238,7 +1237,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>40</v>
       </c>
@@ -1249,7 +1248,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>41</v>
       </c>
@@ -1260,7 +1259,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>42</v>
       </c>
@@ -1271,12 +1270,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>44</v>
       </c>
@@ -1287,7 +1286,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>45</v>
       </c>
@@ -1298,7 +1297,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>46</v>
       </c>
@@ -1310,7 +1309,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>47</v>
       </c>
@@ -1322,7 +1321,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>48</v>
       </c>
@@ -1334,7 +1333,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>49</v>
       </c>
@@ -1346,7 +1345,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>50</v>
       </c>
@@ -1358,29 +1357,29 @@
         <v>83</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>51</v>
       </c>
       <c r="B54" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="C54" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>52</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>53</v>
       </c>
@@ -1391,7 +1390,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>54</v>
       </c>
@@ -1402,18 +1401,18 @@
         <v>83</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>55</v>
       </c>
       <c r="B58" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C58" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>56</v>
       </c>
@@ -1428,72 +1427,72 @@
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B23"/>
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>69</v>
       </c>
@@ -1501,42 +1500,42 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>78</v>
       </c>

</xml_diff>

<commit_message>
GF#22851 change name of device profile to implantable device profile
</commit_message>
<xml_diff>
--- a/source/source_spreadsheets/uscdi_table.xlsx
+++ b/source/source_spreadsheets/uscdi_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ERICS-AIR-2\ehaas\Documents\FHIR\Argo-R4\source\source_spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7706B949-5C70-4216-A639-85AB19E4D562}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55FB8192-7FCB-4EA3-B5AD-43FBA0ED7C9F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="375" yWindow="465" windowWidth="28035" windowHeight="17040" xr2:uid="{AF8CF676-F508-9E49-96CF-11F4326F15E6}"/>
   </bookViews>
@@ -330,9 +330,6 @@
     <t>Immunization</t>
   </si>
   <si>
-    <t>[US Core Device Profile]</t>
-  </si>
-  <si>
     <t>Device</t>
   </si>
   <si>
@@ -412,6 +409,9 @@
   </si>
   <si>
     <t>[US Core Pulse Oximetry Profile]</t>
+  </si>
+  <si>
+    <t>[US Core Implantable Device Profile]</t>
   </si>
 </sst>
 </file>
@@ -796,8 +796,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01009508-76D3-D741-AF15-9B97E20050F9}">
   <dimension ref="A1:C59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -822,10 +822,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C2" t="s">
         <v>101</v>
-      </c>
-      <c r="C2" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -849,10 +849,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>123</v>
+      </c>
+      <c r="C5" t="s">
         <v>124</v>
-      </c>
-      <c r="C5" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -860,10 +860,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>123</v>
+      </c>
+      <c r="C6" t="s">
         <v>124</v>
-      </c>
-      <c r="C6" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -871,10 +871,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>123</v>
+      </c>
+      <c r="C7" t="s">
         <v>124</v>
-      </c>
-      <c r="C7" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -882,10 +882,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>117</v>
+      </c>
+      <c r="C8" t="s">
         <v>118</v>
-      </c>
-      <c r="C8" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -893,10 +893,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>117</v>
+      </c>
+      <c r="C9" t="s">
         <v>118</v>
-      </c>
-      <c r="C9" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -904,10 +904,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>117</v>
+      </c>
+      <c r="C10" t="s">
         <v>118</v>
-      </c>
-      <c r="C10" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -915,10 +915,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>117</v>
+      </c>
+      <c r="C11" t="s">
         <v>118</v>
-      </c>
-      <c r="C11" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -926,10 +926,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>117</v>
+      </c>
+      <c r="C12" t="s">
         <v>118</v>
-      </c>
-      <c r="C12" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -937,10 +937,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
+        <v>123</v>
+      </c>
+      <c r="C13" t="s">
         <v>124</v>
-      </c>
-      <c r="C13" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -948,10 +948,10 @@
         <v>4</v>
       </c>
       <c r="B14" t="s">
+        <v>123</v>
+      </c>
+      <c r="C14" t="s">
         <v>124</v>
-      </c>
-      <c r="C14" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -964,10 +964,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
+        <v>102</v>
+      </c>
+      <c r="C16" t="s">
         <v>103</v>
-      </c>
-      <c r="C16" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1045,7 +1045,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -1058,7 +1058,7 @@
         <v>81</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -1069,7 +1069,7 @@
         <v>81</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -1080,7 +1080,7 @@
         <v>81</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -1091,7 +1091,7 @@
         <v>81</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -1102,7 +1102,7 @@
         <v>81</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -1113,7 +1113,7 @@
         <v>81</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -1124,7 +1124,7 @@
         <v>81</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -1135,7 +1135,7 @@
         <v>81</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -1146,7 +1146,7 @@
         <v>81</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -1157,7 +1157,7 @@
         <v>81</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -1168,7 +1168,7 @@
         <v>81</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -1179,7 +1179,7 @@
         <v>81</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -1209,10 +1209,10 @@
         <v>37</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -1220,10 +1220,10 @@
         <v>38</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -1231,10 +1231,10 @@
         <v>39</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -1242,10 +1242,10 @@
         <v>40</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -1264,10 +1264,10 @@
         <v>42</v>
       </c>
       <c r="B45" t="s">
+        <v>126</v>
+      </c>
+      <c r="C45" t="s">
         <v>99</v>
-      </c>
-      <c r="C45" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -1280,7 +1280,7 @@
         <v>44</v>
       </c>
       <c r="B47" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C47" t="s">
         <v>83</v>
@@ -1291,7 +1291,7 @@
         <v>45</v>
       </c>
       <c r="B48" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C48" t="s">
         <v>83</v>
@@ -1362,7 +1362,7 @@
         <v>51</v>
       </c>
       <c r="B54" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C54" t="s">
         <v>83</v>
@@ -1373,7 +1373,7 @@
         <v>52</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>83</v>
@@ -1384,7 +1384,7 @@
         <v>53</v>
       </c>
       <c r="B56" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C56" t="s">
         <v>83</v>
@@ -1395,7 +1395,7 @@
         <v>54</v>
       </c>
       <c r="B57" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C57" t="s">
         <v>83</v>
@@ -1406,7 +1406,7 @@
         <v>55</v>
       </c>
       <c r="B58" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C58" t="s">
         <v>83</v>

</xml_diff>

<commit_message>
FHIR-26840 remove prov reqs
</commit_message>
<xml_diff>
--- a/source/source_spreadsheets/uscdi_table.xlsx
+++ b/source/source_spreadsheets/uscdi_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ERICS-AIR-2\ehaas\Documents\FHIR\Argo-R4\source\source_spreadsheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ERICS-AIR-2\ehaas\Documents\FHIR\US-Core-R4\source\source_spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55FB8192-7FCB-4EA3-B5AD-43FBA0ED7C9F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D32734C-12D5-408F-8380-70E6AD1BC7AE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="375" yWindow="465" windowWidth="28035" windowHeight="17040" xr2:uid="{AF8CF676-F508-9E49-96CF-11F4326F15E6}"/>
+    <workbookView xWindow="-19320" yWindow="-465" windowWidth="19440" windowHeight="15000" xr2:uid="{AF8CF676-F508-9E49-96CF-11F4326F15E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -231,9 +232,6 @@
     <t>Problems\t[US Core Condition Profile]\tCondition</t>
   </si>
   <si>
-    <t>Medications\t[US Core Medication Profile], [US Core Medication Statement Profile], [US Core Medication Request Profile]\tMedication, MedicationStatement, MedicationRequest</t>
-  </si>
-  <si>
     <t>Medication allergies\t[US Core Allergies Profile]\tAllergyIntolerance</t>
   </si>
   <si>
@@ -291,12 +289,6 @@
     <t>Condition</t>
   </si>
   <si>
-    <t>[US Core Medication Profile], [US Core Medication Statement Profile], [US Core Medication Request Profile]</t>
-  </si>
-  <si>
-    <t>Medication, MedicationStatement, MedicationRequest</t>
-  </si>
-  <si>
     <t>[US Core Allergies Profile]</t>
   </si>
   <si>
@@ -412,6 +404,15 @@
   </si>
   <si>
     <t>[US Core Implantable Device Profile]</t>
+  </si>
+  <si>
+    <t>Medication,  MedicationRequest</t>
+  </si>
+  <si>
+    <t>Medications\t[US Core Medication Profile], [US Core Medication Reqsuest Profile]\tMedication, MedicationRequest</t>
+  </si>
+  <si>
+    <t>[US Core Medication Profile], [US Core Medication Request Profile]</t>
   </si>
 </sst>
 </file>
@@ -796,8 +797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01009508-76D3-D741-AF15-9B97E20050F9}">
   <dimension ref="A1:C59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -811,10 +812,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
@@ -822,10 +823,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -833,10 +834,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -849,10 +850,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C5" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -860,10 +861,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C6" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -871,10 +872,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C7" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -882,10 +883,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C8" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -893,10 +894,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C9" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -904,10 +905,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C10" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -915,10 +916,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C11" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -926,10 +927,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C12" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -937,10 +938,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C13" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -948,10 +949,10 @@
         <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C14" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -964,10 +965,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C16" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -975,10 +976,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
+        <v>83</v>
+      </c>
+      <c r="C17" t="s">
         <v>84</v>
-      </c>
-      <c r="C17" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -986,10 +987,10 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C18" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -1002,7 +1003,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1010,10 +1011,10 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C21" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1026,10 +1027,10 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>86</v>
+        <v>126</v>
       </c>
       <c r="C23" t="s">
-        <v>87</v>
+        <v>124</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -1037,15 +1038,15 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C24" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -1055,10 +1056,10 @@
         <v>23</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -1066,10 +1067,10 @@
         <v>24</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -1077,10 +1078,10 @@
         <v>25</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -1088,10 +1089,10 @@
         <v>26</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -1099,10 +1100,10 @@
         <v>27</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -1110,10 +1111,10 @@
         <v>28</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -1121,10 +1122,10 @@
         <v>29</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -1132,10 +1133,10 @@
         <v>30</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -1143,10 +1144,10 @@
         <v>31</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -1154,10 +1155,10 @@
         <v>32</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -1165,10 +1166,10 @@
         <v>33</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -1176,10 +1177,10 @@
         <v>34</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -1187,10 +1188,10 @@
         <v>35</v>
       </c>
       <c r="B38" t="s">
+        <v>83</v>
+      </c>
+      <c r="C38" t="s">
         <v>84</v>
-      </c>
-      <c r="C38" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -1198,10 +1199,10 @@
         <v>36</v>
       </c>
       <c r="B39" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C39" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -1209,10 +1210,10 @@
         <v>37</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -1220,10 +1221,10 @@
         <v>38</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -1231,10 +1232,10 @@
         <v>39</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -1242,10 +1243,10 @@
         <v>40</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -1253,10 +1254,10 @@
         <v>41</v>
       </c>
       <c r="B44" t="s">
+        <v>81</v>
+      </c>
+      <c r="C44" t="s">
         <v>82</v>
-      </c>
-      <c r="C44" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -1264,10 +1265,10 @@
         <v>42</v>
       </c>
       <c r="B45" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C45" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -1280,10 +1281,10 @@
         <v>44</v>
       </c>
       <c r="B47" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C47" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -1291,10 +1292,10 @@
         <v>45</v>
       </c>
       <c r="B48" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C48" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -1306,7 +1307,7 @@
         <v>[Body height] (From FHIR Core Profiles for Observation)</v>
       </c>
       <c r="C49" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -1318,7 +1319,7 @@
         <v>[Body weight] (From FHIR Core Profiles for Observation)</v>
       </c>
       <c r="C50" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -1330,7 +1331,7 @@
         <v>[Heart rate] (From FHIR Core Profiles for Observation)</v>
       </c>
       <c r="C51" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -1342,7 +1343,7 @@
         <v>[Respiratory rate] (From FHIR Core Profiles for Observation)</v>
       </c>
       <c r="C52" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -1354,7 +1355,7 @@
         <v>[Body temperature] (From FHIR Core Profiles for Observation)</v>
       </c>
       <c r="C53" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -1362,10 +1363,10 @@
         <v>51</v>
       </c>
       <c r="B54" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C54" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -1373,10 +1374,10 @@
         <v>52</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -1384,10 +1385,10 @@
         <v>53</v>
       </c>
       <c r="B56" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C56" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -1395,10 +1396,10 @@
         <v>54</v>
       </c>
       <c r="B57" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C57" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -1406,10 +1407,10 @@
         <v>55</v>
       </c>
       <c r="B58" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C58" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -1427,7 +1428,7 @@
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1479,65 +1480,65 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>66</v>
+        <v>125</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>68</v>
+      </c>
+      <c r="B14" t="s">
         <v>69</v>
-      </c>
-      <c r="B14" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>